<commit_message>
Fix the column mismatch in the prod prediction
</commit_message>
<xml_diff>
--- a/data/processed/admission/app_test_dataset.xlsx
+++ b/data/processed/admission/app_test_dataset.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luis.serna\Documents\Github\ds4a-team-62\data\processed\admission\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Synced_PCs\github\ds4a-team-62\data\processed\admission\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DACE79E3-0B42-47E3-9074-299D6E285516}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EACBEF7B-9484-4258-B946-9E63428688ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -26,9 +26,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
@@ -417,7 +415,7 @@
   <dimension ref="A1:P50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1802,7 +1800,7 @@
         <v>6</v>
       </c>
       <c r="I28">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J28">
         <v>1</v>
@@ -2352,7 +2350,7 @@
         <v>1</v>
       </c>
       <c r="I39">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J39">
         <v>1</v>

</xml_diff>

<commit_message>
add charts descriptive analytics
</commit_message>
<xml_diff>
--- a/data/processed/admission/app_test_dataset.xlsx
+++ b/data/processed/admission/app_test_dataset.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luis.serna\Documents\Github\ds4a-team-62\data\processed\admission\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DB985AA-3733-4924-A877-CDD1CEE83275}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FA0D851-F05C-4CB3-B9A2-D63DCED7877C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -414,7 +414,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:P50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -577,7 +579,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -677,7 +679,7 @@
         <v>1</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -827,7 +829,7 @@
         <v>2</v>
       </c>
       <c r="B9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -1027,7 +1029,7 @@
         <v>1</v>
       </c>
       <c r="B13">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C13">
         <v>0</v>
@@ -1177,7 +1179,7 @@
         <v>2</v>
       </c>
       <c r="B16">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -1277,7 +1279,7 @@
         <v>1</v>
       </c>
       <c r="B18">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C18">
         <v>0</v>
@@ -1377,7 +1379,7 @@
         <v>3</v>
       </c>
       <c r="B20">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C20">
         <v>1</v>
@@ -1427,7 +1429,7 @@
         <v>1</v>
       </c>
       <c r="B21">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C21">
         <v>1</v>
@@ -1477,7 +1479,7 @@
         <v>1</v>
       </c>
       <c r="B22">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C22">
         <v>1</v>
@@ -1727,7 +1729,7 @@
         <v>1</v>
       </c>
       <c r="B27">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C27">
         <v>1</v>
@@ -1877,7 +1879,7 @@
         <v>1</v>
       </c>
       <c r="B30">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C30">
         <v>1</v>
@@ -1977,7 +1979,7 @@
         <v>2</v>
       </c>
       <c r="B32">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C32">
         <v>1</v>
@@ -2077,7 +2079,7 @@
         <v>3</v>
       </c>
       <c r="B34">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C34">
         <v>1</v>
@@ -2177,7 +2179,7 @@
         <v>2</v>
       </c>
       <c r="B36">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C36">
         <v>1</v>
@@ -2627,7 +2629,7 @@
         <v>1</v>
       </c>
       <c r="B45">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C45">
         <v>1</v>
@@ -2727,7 +2729,7 @@
         <v>1</v>
       </c>
       <c r="B47">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C47">
         <v>0</v>
@@ -2777,7 +2779,7 @@
         <v>1</v>
       </c>
       <c r="B48">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C48">
         <v>1</v>
@@ -2827,7 +2829,7 @@
         <v>1</v>
       </c>
       <c r="B49">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C49">
         <v>1</v>
@@ -2876,7 +2878,6 @@
       <c r="M50" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:P49" xr:uid="{00000000-0001-0000-0100-000000000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:P50">
     <sortCondition ref="B2:B50"/>
   </sortState>

</xml_diff>